<commit_message>
Add statistics with writing to db, using postgrel and hibernate
</commit_message>
<xml_diff>
--- a/phoneBase/base.xlsx
+++ b/phoneBase/base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oleksii.vasylenko\OneDrive - Proximaresearch International LLC\Документи\IdeaProjects\ProximaSFTPconnect_v.2.1_logger\phoneBase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oleksii.vasylenko\OneDrive - Proximaresearch International LLC\Документи\IdeaProjects\Proxima.v.3.0\phoneBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EB7B8C-4A1B-47C9-B2FE-E5545385BCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2485FC7-E343-45A5-9E5F-F61FBE940437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="0" windowWidth="9540" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Рабочий</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>Head of Heads</t>
+  </si>
+  <si>
+    <t>+380664770142</t>
+  </si>
+  <si>
+    <t>Вася Столяренко 2</t>
+  </si>
+  <si>
+    <t>Никита Алферов</t>
+  </si>
+  <si>
+    <t>+380632481387</t>
   </si>
 </sst>
 </file>
@@ -434,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -570,6 +582,22 @@
         <v>27</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix bug with db writing. Add 'working time' feature in db entity
</commit_message>
<xml_diff>
--- a/phoneBase/base.xlsx
+++ b/phoneBase/base.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oleksii.vasylenko\OneDrive - Proximaresearch International LLC\Документи\IdeaProjects\Proxima.v.3.0\phoneBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2485FC7-E343-45A5-9E5F-F61FBE940437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCEF0D0-925B-4386-B3CA-A16B67CC9306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="0" windowWidth="9540" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Рабочий</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>+380632481387</t>
+  </si>
+  <si>
+    <t>Маша Тестировщик</t>
+  </si>
+  <si>
+    <t>+380954121725</t>
   </si>
 </sst>
 </file>
@@ -446,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -598,6 +604,14 @@
         <v>33</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>